<commit_message>
Define build_type 2 as office building. #2
</commit_message>
<xml_diff>
--- a/pycity_calc/data/BaseData/Specific_Demand_Data/Spec_demands_non_res.xlsx
+++ b/pycity_calc/data/BaseData/Specific_Demand_Data/Spec_demands_non_res.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pyCity_calc\pycity_calc\data\BaseData\Specific_Demand_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="13350"/>
   </bookViews>
@@ -171,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -705,14 +710,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -750,9 +758,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -787,7 +795,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -822,7 +830,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -998,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1041,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1053,7 +1061,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -1072,8 +1080,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" s="1">
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1093,7 +1101,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1113,7 +1121,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -1133,7 +1141,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -1153,7 +1161,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -1173,7 +1181,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1193,7 +1201,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -1213,7 +1221,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -1233,7 +1241,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -1253,7 +1261,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -1273,7 +1281,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1293,7 +1301,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
@@ -1313,7 +1321,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
@@ -1333,7 +1341,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
@@ -1353,7 +1361,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -1373,7 +1381,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
@@ -1393,7 +1401,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
@@ -1413,7 +1421,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
@@ -1433,7 +1441,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
@@ -1453,7 +1461,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
@@ -1473,7 +1481,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>24</v>
@@ -1493,7 +1501,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>25</v>
@@ -1513,7 +1521,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>26</v>
@@ -1533,7 +1541,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
@@ -1553,7 +1561,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
@@ -1573,7 +1581,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>29</v>
@@ -1593,7 +1601,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>30</v>
@@ -1613,7 +1621,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>31</v>
@@ -1633,7 +1641,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>32</v>
@@ -1653,7 +1661,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>33</v>
@@ -1673,7 +1681,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>34</v>
@@ -1693,7 +1701,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>35</v>
@@ -1713,7 +1721,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>36</v>
@@ -1733,7 +1741,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>37</v>
@@ -1753,7 +1761,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>38</v>
@@ -1773,7 +1781,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>39</v>
@@ -1793,7 +1801,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>40</v>
@@ -1813,7 +1821,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>41</v>
@@ -1833,7 +1841,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>42</v>
@@ -1853,7 +1861,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>43</v>
@@ -1873,7 +1881,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>44</v>
@@ -1892,8 +1900,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>44</v>
+      <c r="A45">
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Translate German terms into English language #2
</commit_message>
<xml_diff>
--- a/pycity_calc/data/BaseData/Specific_Demand_Data/Spec_demands_non_res.xlsx
+++ b/pycity_calc/data/BaseData/Specific_Demand_Data/Spec_demands_non_res.xlsx
@@ -29,148 +29,148 @@
     <t>type_name</t>
   </si>
   <si>
-    <t>Bauhauptgewerbe</t>
-  </si>
-  <si>
-    <t>Ausbaugewerbe</t>
-  </si>
-  <si>
-    <t>Banken, Versicherung</t>
-  </si>
-  <si>
-    <t>Oeffentl. Einrichtungen</t>
-  </si>
-  <si>
-    <t>Org. ohne Erwerbszweck</t>
-  </si>
-  <si>
-    <t>Kleine Bueros</t>
-  </si>
-  <si>
-    <t>Sonst. Dienstleistungen</t>
-  </si>
-  <si>
     <t>Metall</t>
   </si>
   <si>
-    <t>KFZ</t>
-  </si>
-  <si>
-    <t>Holz</t>
-  </si>
-  <si>
-    <t>Papier</t>
-  </si>
-  <si>
-    <t>Einzelhandel Lebensmittel</t>
-  </si>
-  <si>
-    <t>Einzelhandel Non-food</t>
-  </si>
-  <si>
-    <t>Großhandel Lebensmittel</t>
-  </si>
-  <si>
-    <t>Grosshandel Non-food</t>
-  </si>
-  <si>
-    <t>Grund-/Hauptschule</t>
-  </si>
-  <si>
-    <t>Behindertenschule</t>
-  </si>
-  <si>
-    <t>Realschule/Gymnasium</t>
-  </si>
-  <si>
-    <t>Berufsschule</t>
-  </si>
-  <si>
-    <t>Hochschule</t>
-  </si>
-  <si>
     <t>Hotels</t>
   </si>
   <si>
-    <t>Gaststaetten</t>
-  </si>
-  <si>
-    <t>Heim</t>
-  </si>
-  <si>
-    <t>Baeckerei</t>
-  </si>
-  <si>
-    <t>Fleischerei</t>
-  </si>
-  <si>
-    <t>Waescherei</t>
-  </si>
-  <si>
-    <t>Ueberwiegend Ackerbau</t>
-  </si>
-  <si>
-    <t>Mischbetriebe 10 - 49 GVE</t>
-  </si>
-  <si>
-    <t>Mischbetriebe 50 - 100 GVE</t>
-  </si>
-  <si>
-    <t>Viehhaltung &gt; 100 GVE</t>
-  </si>
-  <si>
-    <t>Gartenbau</t>
-  </si>
-  <si>
-    <t>Krankenhaus</t>
-  </si>
-  <si>
-    <t>Bibliotheksgebaeude</t>
-  </si>
-  <si>
-    <t>Gefaengnisse</t>
-  </si>
-  <si>
-    <t>Kino</t>
-  </si>
-  <si>
-    <t>Theater, Oper</t>
-  </si>
-  <si>
-    <t>Jugendhaeuser, Gemeindehaeuser</t>
-  </si>
-  <si>
-    <t>Sporthalle</t>
-  </si>
-  <si>
-    <t>Mehrzweckhalle</t>
-  </si>
-  <si>
-    <t>Schwimmhalle</t>
-  </si>
-  <si>
-    <t>Sportheim, Vereinsheim</t>
-  </si>
-  <si>
-    <t>Fitnessstudio</t>
-  </si>
-  <si>
-    <t>Bahnhof &lt; 5000m2</t>
-  </si>
-  <si>
-    <t>Bahnhof &gt;= 5000m2</t>
-  </si>
-  <si>
-    <t>Spez. Stromverbrauch kWh/m2*a</t>
-  </si>
-  <si>
-    <t>Spez. Brennstoffverbrauch kWh/m2*a</t>
-  </si>
-  <si>
     <t>SLP_th_type</t>
   </si>
   <si>
     <t>SLP_el_type</t>
+  </si>
+  <si>
+    <t>Spec.final th. energy demand in kWh/m2*a</t>
+  </si>
+  <si>
+    <t>Spec. el. energy demand kWh/m2*a</t>
+  </si>
+  <si>
+    <t>bank and insurance</t>
+  </si>
+  <si>
+    <t>Non profit organizations</t>
+  </si>
+  <si>
+    <t>Small office buildings</t>
+  </si>
+  <si>
+    <t>Other services</t>
+  </si>
+  <si>
+    <t>Public institutions</t>
+  </si>
+  <si>
+    <t>Finishing trade construction work</t>
+  </si>
+  <si>
+    <t>Main construction work</t>
+  </si>
+  <si>
+    <t>Automobile</t>
+  </si>
+  <si>
+    <t>Wood and timber</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Small retailer for food</t>
+  </si>
+  <si>
+    <t>Small retailer for non-food</t>
+  </si>
+  <si>
+    <t>Large retailer for food</t>
+  </si>
+  <si>
+    <t>Large retailer for non-food</t>
+  </si>
+  <si>
+    <t>Primary school</t>
+  </si>
+  <si>
+    <t>School for physically handicapped</t>
+  </si>
+  <si>
+    <t>High school</t>
+  </si>
+  <si>
+    <t>Trade school</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Restaurants</t>
+  </si>
+  <si>
+    <t>Childrens home</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t>Backery</t>
+  </si>
+  <si>
+    <t>Laundry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farm primary agriculture </t>
+  </si>
+  <si>
+    <t>Farm with 10 - 49 cattle units</t>
+  </si>
+  <si>
+    <t>Farm with 50 - 100 cattle units</t>
+  </si>
+  <si>
+    <t>Farm with more than 100 cattle units</t>
+  </si>
+  <si>
+    <t>Gardening</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Prison</t>
+  </si>
+  <si>
+    <t>Cinema</t>
+  </si>
+  <si>
+    <t>Theater</t>
+  </si>
+  <si>
+    <t>Parish hall</t>
+  </si>
+  <si>
+    <t>Sports hall</t>
+  </si>
+  <si>
+    <t>Multi purpose hall</t>
+  </si>
+  <si>
+    <t>Swimming hall</t>
+  </si>
+  <si>
+    <t>Club house</t>
+  </si>
+  <si>
+    <t>Fitness studio</t>
+  </si>
+  <si>
+    <t>Train station smaller 5000m2</t>
+  </si>
+  <si>
+    <t>Train station equal or larger than 5000m2</t>
   </si>
 </sst>
 </file>
@@ -1006,15 +1006,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1027,16 +1027,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
         <v>22.96</v>
@@ -1064,7 +1064,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
         <v>28.66</v>
@@ -1084,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>49.69</v>
@@ -1104,7 +1104,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>40.07</v>
@@ -1124,7 +1124,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
         <v>50.23</v>
@@ -1144,7 +1144,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
         <v>5.6</v>
@@ -1164,7 +1164,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
         <v>75.86</v>
@@ -1184,7 +1184,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
         <v>55.44</v>
@@ -1204,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2">
         <v>26.31</v>
@@ -1224,7 +1224,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <v>37.880000000000003</v>
@@ -1244,7 +1244,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2">
         <v>92.18</v>
@@ -1264,7 +1264,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2">
         <v>145.58000000000001</v>
@@ -1284,7 +1284,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2">
         <v>32.71</v>
@@ -1304,7 +1304,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2">
         <v>48.43</v>
@@ -1324,7 +1324,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2">
         <v>38.79</v>
@@ -1344,7 +1344,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2">
         <v>102.08</v>
@@ -1364,7 +1364,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2">
         <v>92.73</v>
@@ -1384,7 +1384,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2">
         <v>168.49</v>
@@ -1404,7 +1404,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2">
         <v>97.39</v>
@@ -1424,7 +1424,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2">
         <v>160.12</v>
@@ -1444,7 +1444,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C22" s="2">
         <v>172.9</v>
@@ -1464,7 +1464,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2">
         <v>259.75</v>
@@ -1484,7 +1484,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2">
         <v>122.81</v>
@@ -1504,7 +1504,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2">
         <v>403.95</v>
@@ -1524,7 +1524,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C26" s="2">
         <v>182.95</v>
@@ -1544,7 +1544,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C27" s="2">
         <v>471.59</v>
@@ -1564,7 +1564,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2">
         <v>1136.17</v>
@@ -1584,7 +1584,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2">
         <v>710.87</v>
@@ -1604,7 +1604,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2">
         <v>196.32</v>
@@ -1624,7 +1624,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C31" s="2">
         <v>251.41</v>
@@ -1644,7 +1644,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2">
         <v>2688</v>
@@ -1664,7 +1664,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C33" s="2">
         <v>192.13</v>
@@ -1684,7 +1684,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C34" s="2">
         <v>80</v>
@@ -1704,7 +1704,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C35" s="2">
         <v>260</v>
@@ -1724,7 +1724,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C36" s="2">
         <v>80</v>
@@ -1744,7 +1744,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C37" s="2">
         <v>155</v>
@@ -1764,7 +1764,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C38" s="2">
         <v>150</v>
@@ -1784,7 +1784,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C39" s="2">
         <v>170</v>
@@ -1804,7 +1804,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C40" s="2">
         <v>345</v>
@@ -1824,7 +1824,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C41" s="2">
         <v>550</v>
@@ -1844,7 +1844,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C42" s="2">
         <v>115</v>
@@ -1864,7 +1864,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C43" s="2">
         <v>140</v>
@@ -1884,7 +1884,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C44" s="2">
         <v>170</v>
@@ -1904,7 +1904,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C45" s="2">
         <v>165</v>

</xml_diff>